<commit_message>
employee utilization reporting and issues fixes, notification for project create.
</commit_message>
<xml_diff>
--- a/Base/src/main/resources/templates/team2.xlsx
+++ b/Base/src/main/resources/templates/team2.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Project Report" sheetId="1" r:id="rId1"/>
+    <sheet name="Emp Utilization" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Read Me</t>
   </si>
@@ -66,6 +67,9 @@
   </si>
   <si>
     <t>Analyst Comments</t>
+  </si>
+  <si>
+    <t>Employees</t>
   </si>
 </sst>
 </file>
@@ -75,7 +79,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\-mm\-yy"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,8 +111,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -133,8 +145,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -187,12 +205,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -211,6 +240,9 @@
     <xf numFmtId="164" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -690,4 +722,27 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>